<commit_message>
Complete Power BI dashboard & Report of Excel
</commit_message>
<xml_diff>
--- a/Reports/Shopping Analysis Report.xlsx
+++ b/Reports/Shopping Analysis Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\Shopping Analysis\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42BAF73-69BC-4E03-90E9-6C0894BEE588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5D38F3-812E-4A8B-BF38-D2B439C6DA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{91B29881-4FC9-4F76-940C-C5551F218297}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="130">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -456,27 +456,15 @@
     <t>Tells how much on average each customer spends — helps understand customer value.</t>
   </si>
   <si>
-    <t>Average Spending = DIVIDE(SUM('Shopping_Data'[Total Amount]), DISTINCTCOUNT('Shopping_Data'[Customer ID]))</t>
-  </si>
-  <si>
     <t>Average Basket Size</t>
   </si>
   <si>
     <t>Measures the average number of items (quantity) purchased per customer — helps understand purchase behavior.</t>
   </si>
   <si>
-    <t>Average Basket Size = DIVIDE(SUM('Shopping_Data'[Quantity]), DISTINCTCOUNT('Shopping_Data'[Customer ID]))</t>
-  </si>
-  <si>
     <t>Online vs Offline Sales %</t>
   </si>
   <si>
-    <t>Compares total revenue from online payments (Credit/Debit Card, UPI) vs offline payments (Cash) — shows payment trend.</t>
-  </si>
-  <si>
-    <t>Online Sales % = DIVIDE(SUMX(FILTER('Shopping_Data', 'Shopping_Data'[Payment Type Category] = "Online"), 'Shopping_Data'[Total Amount]), SUM('Shopping_Data'[Total Amount])) * 100Offline Sales % = 100 - [Online Sales %]</t>
-  </si>
-  <si>
     <t>Visual Type</t>
   </si>
   <si>
@@ -504,15 +492,6 @@
     <t>Understand revenue contribution by each product category.</t>
   </si>
   <si>
-    <t>Customer ID, Quantity</t>
-  </si>
-  <si>
-    <t>Card / KPI Visual</t>
-  </si>
-  <si>
-    <t>Displays average number of items purchased per customer.</t>
-  </si>
-  <si>
     <t>Age Group Distribution</t>
   </si>
   <si>
@@ -546,18 +525,6 @@
     <t>Shows revenue trends month by month for time-based analysis.</t>
   </si>
   <si>
-    <t>Top Customers by Spending</t>
-  </si>
-  <si>
-    <t>Customer ID, Total Amount</t>
-  </si>
-  <si>
-    <t>Bar Chart / Table</t>
-  </si>
-  <si>
-    <t>Identify high-value customers based on total spend.</t>
-  </si>
-  <si>
     <t>Payment Method Analysis</t>
   </si>
   <si>
@@ -567,9 +534,6 @@
     <t>Displays popularity of each payment mode (Cash, Credit, Debit).</t>
   </si>
   <si>
-    <t>Date Filter / Slicer</t>
-  </si>
-  <si>
     <t>Mall Filter</t>
   </si>
   <si>
@@ -582,10 +546,47 @@
     <t>Age Group Filter</t>
   </si>
   <si>
-    <t>Payment Type Filter</t>
-  </si>
-  <si>
     <t>Payment Method Filter</t>
+  </si>
+  <si>
+    <t>Average Spending = DIVIDE(
+    SUM(customer_shopping_data[Total Amount]), 
+    DISTINCTCOUNT(customer_shopping_data[Customer ID])
+)</t>
+  </si>
+  <si>
+    <t>Average Basket Size = DIVIDE(
+    SUM('customer_shopping_data'[Quantity]), 
+    DISTINCTCOUNT('customer_shopping_data'[Customer ID])
+)</t>
+  </si>
+  <si>
+    <t>Offline Sales % = 100 - [Online Sales %]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offline Sales % </t>
+  </si>
+  <si>
+    <t>Compares total revenue from offline payments  (Cash) — shows payment trend.</t>
+  </si>
+  <si>
+    <t>Compares total revenue from online payments (Credit/Debit Card, UPI) shows payment trend.</t>
+  </si>
+  <si>
+    <t>Online Sales %</t>
+  </si>
+  <si>
+    <t>Online Sales % = 
+DIVIDE(
+    SUMX(
+        FILTER(
+            'Shopping_Data', 
+            'Shopping_Data'[Payment Method] = "Online"
+        ), 
+        'Shopping_Data'[Total Amount]
+    ), 
+    SUM('Shopping_Data'[Total Amount])
+) * 100</t>
   </si>
 </sst>
 </file>
@@ -742,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -785,7 +786,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -793,6 +793,13 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1129,7 +1136,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="25.8">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1424,15 +1431,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="25.8">
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="21">
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1707,7 +1714,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629CA377-913D-4D87-B292-24EAC4E976A2}">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -1721,7 +1728,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="25.8">
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1779,9 +1786,6 @@
       <c r="D8" s="17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="C9" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1790,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB7041C-421E-42FE-B3DC-0F9770F9E209}">
-  <dimension ref="B2:S12"/>
+  <dimension ref="B2:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1852,7 +1856,7 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>39</v>
@@ -1877,35 +1881,35 @@
       <c r="F5" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>88</v>
       </c>
       <c r="J5" s="18">
         <v>1</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>99</v>
+      <c r="K5" s="26" t="s">
+        <v>95</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="18">
         <v>1</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" ht="31.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="52.8">
       <c r="D6" s="18">
         <v>2</v>
       </c>
@@ -1915,203 +1919,163 @@
       <c r="F6" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>91</v>
+      <c r="G6" s="23" t="s">
+        <v>122</v>
       </c>
       <c r="J6" s="18">
         <v>2</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>103</v>
+      <c r="K6" s="26" t="s">
+        <v>99</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Q6" s="18">
         <v>2</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="S6" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" ht="46.8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="52.8">
       <c r="D7" s="18">
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>94</v>
+      <c r="G7" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="J7" s="18">
         <v>3</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>92</v>
+      <c r="K7" s="26" t="s">
+        <v>103</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Q7" s="18">
         <v>3</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" ht="52.8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="145.19999999999999">
       <c r="D8" s="18">
         <v>4</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>97</v>
+        <v>127</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="J8" s="18">
         <v>4</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>110</v>
+      <c r="K8" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q8" s="18">
         <v>4</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="S8" s="17" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="31.2">
+      <c r="D9" s="18">
+        <v>5</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="J9" s="18">
         <v>5</v>
       </c>
-      <c r="K9" s="17" t="s">
-        <v>95</v>
+      <c r="K9" s="26" t="s">
+        <v>110</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="Q9" s="18">
         <v>5</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="S9" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="31.2">
       <c r="J10" s="18">
         <v>6</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>117</v>
+      <c r="K10" s="26" t="s">
+        <v>114</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q10" s="18">
-        <v>6</v>
-      </c>
-      <c r="R10" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="S10" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="31.2">
-      <c r="J11" s="18">
-        <v>7</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q11" s="18">
-        <v>7</v>
-      </c>
-      <c r="R11" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="S11" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" ht="31.2">
-      <c r="J12" s="18">
-        <v>8</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>